<commit_message>
Can save warning setting even after shutting down
</commit_message>
<xml_diff>
--- a/lot-tracker-test.xlsx
+++ b/lot-tracker-test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -37,97 +37,34 @@
     <t xml:space="preserve">Onion</t>
   </si>
   <si>
-    <t xml:space="preserve">JASKJ09384</t>
-  </si>
-  <si>
     <t xml:space="preserve">Garlic</t>
   </si>
   <si>
-    <t xml:space="preserve">NCAJ8453</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sugar</t>
   </si>
   <si>
-    <t xml:space="preserve">123ABC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Salt</t>
   </si>
   <si>
-    <t xml:space="preserve">123456</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pepper</t>
   </si>
   <si>
-    <t xml:space="preserve">NASJ41.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syrup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASJ-392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red Pepper Flakes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QWIC9831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celery Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93278ANCKJEHF10923CNAJE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celery Powder 123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9318-20349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HFERYE123432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cucumber</t>
-  </si>
-  <si>
-    <t>JASKJ09384</t>
-  </si>
-  <si>
-    <t>NCAJ8453</t>
-  </si>
-  <si>
-    <t>123ABC</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>NASJ41.12</t>
-  </si>
-  <si>
-    <t>ASJ-392</t>
-  </si>
-  <si>
-    <t>QWIC9831</t>
-  </si>
-  <si>
-    <t>93278ANCKJEHF10923CNAJE</t>
-  </si>
-  <si>
-    <t>9318-20349</t>
-  </si>
-  <si>
-    <t>HFERYE123432</t>
-  </si>
-  <si>
-    <t>q230495wergnweg</t>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>231234r</t>
+  </si>
+  <si>
+    <t>23ifw45gw34</t>
+  </si>
+  <si>
+    <t>qw23j3q45t</t>
+  </si>
+  <si>
+    <t>q239o83q4gw5g</t>
+  </si>
+  <si>
+    <t>2w34u9gw45</t>
   </si>
 </sst>
 </file>
@@ -137,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -179,13 +116,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -231,7 +161,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,10 +175,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,10 +198,10 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.86" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="17.4" collapsed="true" outlineLevel="0"/>
@@ -289,13 +215,16 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -304,8 +233,8 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>25</v>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,10 +242,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,10 +253,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,10 +264,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,75 +275,18 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Made it clearer to user that they can get rid of the warning
</commit_message>
<xml_diff>
--- a/lot-tracker-test.xlsx
+++ b/lot-tracker-test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -198,10 +198,10 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.86" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="17.4" collapsed="true" outlineLevel="0"/>

</xml_diff>